<commit_message>
Added Husky and Fetch xyyaw figs and updated figure sizes in chapter 6
</commit_message>
<xml_diff>
--- a/tables/final_compiled_test_results_and_figs.xlsx
+++ b/tables/final_compiled_test_results_and_figs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="8145" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="8145" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fetch_Nav" sheetId="1" r:id="rId1"/>
@@ -1129,11 +1129,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-677948192"/>
-        <c:axId val="-677943840"/>
+        <c:axId val="-1495968832"/>
+        <c:axId val="-1495967744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-677948192"/>
+        <c:axId val="-1495968832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -1174,7 +1174,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:ln>
                       <a:noFill/>
                     </a:ln>
@@ -1184,18 +1184,21 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Garamond" panose="02020404030301010803" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200" b="1">
+                    <a:latin typeface="Garamond" panose="02020404030301010803" pitchFamily="18" charset="0"/>
+                  </a:rPr>
                   <a:t>Distance From Start (m)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1209,7 +1212,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
@@ -1219,7 +1222,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Garamond" panose="02020404030301010803" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -1268,12 +1271,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-677943840"/>
+        <c:crossAx val="-1495967744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-677943840"/>
+        <c:axId val="-1495967744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -1314,7 +1317,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:ln>
                       <a:noFill/>
                     </a:ln>
@@ -1324,18 +1327,21 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Garamond" panose="02020404030301010803" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200" b="1">
+                    <a:latin typeface="Garamond" panose="02020404030301010803" pitchFamily="18" charset="0"/>
+                  </a:rPr>
                   <a:t> Error (cm)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1349,7 +1355,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
@@ -1359,7 +1365,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Garamond" panose="02020404030301010803" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -1408,7 +1414,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-677948192"/>
+        <c:crossAx val="-1495968832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1446,6 +1452,7 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1459,7 +1466,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -1469,7 +1476,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Garamond" panose="02020404030301010803" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -2246,11 +2253,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-677947648"/>
-        <c:axId val="-677950368"/>
+        <c:axId val="-1495961760"/>
+        <c:axId val="-1495957952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-677947648"/>
+        <c:axId val="-1495961760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -2318,6 +2325,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2384,12 +2392,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-677950368"/>
+        <c:crossAx val="-1495957952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-677950368"/>
+        <c:axId val="-1495957952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -2451,6 +2459,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2517,7 +2526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-677947648"/>
+        <c:crossAx val="-1495961760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2555,6 +2564,7 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2996,11 +3006,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-677952000"/>
-        <c:axId val="-677944384"/>
+        <c:axId val="-1495959040"/>
+        <c:axId val="-1495966112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-677952000"/>
+        <c:axId val="-1495959040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -3068,6 +3078,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3134,12 +3145,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-677944384"/>
+        <c:crossAx val="-1495966112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-677944384"/>
+        <c:axId val="-1495966112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -3201,6 +3212,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3267,7 +3279,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-677952000"/>
+        <c:crossAx val="-1495959040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3293,6 +3305,7 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3734,11 +3747,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-905679456"/>
-        <c:axId val="-720721776"/>
+        <c:axId val="-1495963936"/>
+        <c:axId val="-1495965024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-905679456"/>
+        <c:axId val="-1495963936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -3800,6 +3813,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3866,12 +3880,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-720721776"/>
+        <c:crossAx val="-1495965024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-720721776"/>
+        <c:axId val="-1495965024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -3933,6 +3947,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3999,7 +4014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-905679456"/>
+        <c:crossAx val="-1495963936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4025,6 +4040,7 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6106,11 +6122,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674287808"/>
-        <c:axId val="-674287264"/>
+        <c:axId val="-1495972640"/>
+        <c:axId val="-1495973184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-674287808"/>
+        <c:axId val="-1495972640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7"/>
@@ -6238,12 +6254,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674287264"/>
+        <c:crossAx val="-1495973184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674287264"/>
+        <c:axId val="-1495973184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -6379,7 +6395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674287808"/>
+        <c:crossAx val="-1495972640"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7637,11 +7653,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674286176"/>
-        <c:axId val="-674289440"/>
+        <c:axId val="-1350942768"/>
+        <c:axId val="-1350943312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-674286176"/>
+        <c:axId val="-1350942768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -7769,12 +7785,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674289440"/>
+        <c:crossAx val="-1350943312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674289440"/>
+        <c:axId val="-1350943312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="225"/>
@@ -7911,7 +7927,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674286176"/>
+        <c:crossAx val="-1350942768"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -9437,11 +9453,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674295968"/>
-        <c:axId val="-674285088"/>
+        <c:axId val="-1350951472"/>
+        <c:axId val="-1350954192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-674295968"/>
+        <c:axId val="-1350951472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -9570,12 +9586,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674285088"/>
+        <c:crossAx val="-1350954192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674285088"/>
+        <c:axId val="-1350954192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18"/>
@@ -9713,7 +9729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674295968"/>
+        <c:crossAx val="-1350951472"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11251,11 +11267,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674284000"/>
-        <c:axId val="-674283456"/>
+        <c:axId val="-1350943856"/>
+        <c:axId val="-1350949840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-674284000"/>
+        <c:axId val="-1350943856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -11384,12 +11400,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674283456"/>
+        <c:crossAx val="-1350949840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674283456"/>
+        <c:axId val="-1350949840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -11527,7 +11543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674284000"/>
+        <c:crossAx val="-1350943856"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16635,24 +16651,24 @@
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17747,24 +17763,24 @@
       <selection activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18865,8 +18881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="W39" sqref="W39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19092,20 +19108,19 @@
       <selection activeCell="AG20" sqref="AG20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9"/>
     <col min="16" max="16" width="9"/>
-    <col min="23" max="23" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -34820,16 +34835,16 @@
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -42833,32 +42848,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="Q7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.125" customWidth="1"/>
-    <col min="2" max="2" width="39.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" customWidth="1"/>
-    <col min="6" max="7" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="9.125" customWidth="1"/>
-    <col min="16" max="16" width="39.75" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="36" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Updated tables to include mean values and bolded important numbers
</commit_message>
<xml_diff>
--- a/tables/final_compiled_test_results_and_figs.xlsx
+++ b/tables/final_compiled_test_results_and_figs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="65">
   <si>
     <t>5m</t>
   </si>
@@ -232,12 +232,19 @@
     <numFmt numFmtId="165" formatCode="0.0_ "/>
     <numFmt numFmtId="166" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -290,14 +297,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -318,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -330,22 +337,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1129,11 +1142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="413509840"/>
-        <c:axId val="413510384"/>
+        <c:axId val="-229806880"/>
+        <c:axId val="-229816128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="413509840"/>
+        <c:axId val="-229806880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -1271,12 +1284,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413510384"/>
+        <c:crossAx val="-229816128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="413510384"/>
+        <c:axId val="-229816128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -1414,7 +1427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413509840"/>
+        <c:crossAx val="-229806880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2253,11 +2266,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="413514192"/>
-        <c:axId val="413506032"/>
+        <c:axId val="-229813952"/>
+        <c:axId val="-229809056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="413514192"/>
+        <c:axId val="-229813952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -2392,12 +2405,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413506032"/>
+        <c:crossAx val="-229809056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="413506032"/>
+        <c:axId val="-229809056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -2526,7 +2539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413514192"/>
+        <c:crossAx val="-229813952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3006,11 +3019,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="413503856"/>
-        <c:axId val="413512560"/>
+        <c:axId val="-229817216"/>
+        <c:axId val="-229803072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="413503856"/>
+        <c:axId val="-229817216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -3145,12 +3158,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413512560"/>
+        <c:crossAx val="-229803072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="413512560"/>
+        <c:axId val="-229803072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -3279,7 +3292,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413503856"/>
+        <c:crossAx val="-229817216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3747,11 +3760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="413502224"/>
-        <c:axId val="413514736"/>
+        <c:axId val="-229815584"/>
+        <c:axId val="-229814496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="413502224"/>
+        <c:axId val="-229815584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -3880,12 +3893,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413514736"/>
+        <c:crossAx val="-229814496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="413514736"/>
+        <c:axId val="-229814496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -4014,7 +4027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413502224"/>
+        <c:crossAx val="-229815584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6122,11 +6135,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="413500592"/>
-        <c:axId val="413501136"/>
+        <c:axId val="-231330304"/>
+        <c:axId val="-84761952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="413500592"/>
+        <c:axId val="-231330304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7"/>
@@ -6255,12 +6268,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413501136"/>
+        <c:crossAx val="-84761952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="413501136"/>
+        <c:axId val="-84761952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -6397,7 +6410,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413500592"/>
+        <c:crossAx val="-231330304"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7656,11 +7669,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177016464"/>
-        <c:axId val="177017552"/>
+        <c:axId val="-84761408"/>
+        <c:axId val="-84755968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177016464"/>
+        <c:axId val="-84761408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -7789,12 +7802,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177017552"/>
+        <c:crossAx val="-84755968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177017552"/>
+        <c:axId val="-84755968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="225"/>
@@ -7932,7 +7945,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177016464"/>
+        <c:crossAx val="-84761408"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -9459,11 +9472,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177018096"/>
-        <c:axId val="177018640"/>
+        <c:axId val="-84754880"/>
+        <c:axId val="-84760864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177018096"/>
+        <c:axId val="-84754880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -9592,12 +9605,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177018640"/>
+        <c:crossAx val="-84760864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177018640"/>
+        <c:axId val="-84760864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18"/>
@@ -9698,7 +9711,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -9735,7 +9748,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177018096"/>
+        <c:crossAx val="-84754880"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11273,11 +11286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="419785504"/>
-        <c:axId val="419787136"/>
+        <c:axId val="-84759232"/>
+        <c:axId val="-84758688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="419785504"/>
+        <c:axId val="-84759232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -11406,12 +11419,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419787136"/>
+        <c:crossAx val="-84758688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="419787136"/>
+        <c:axId val="-84758688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -11512,7 +11525,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11549,7 +11562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419785504"/>
+        <c:crossAx val="-84759232"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16651,10 +16664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U34"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="L31" sqref="L31:R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -16679,21 +16692,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
@@ -17748,6 +17761,35 @@
       <c r="R34" s="12">
         <f t="shared" si="4"/>
         <v>1.9870790260500214E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="12:18">
+      <c r="L35" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="12">
+        <f>AVERAGE(M32:M34)</f>
+        <v>4.665</v>
+      </c>
+      <c r="N35" s="12">
+        <f t="shared" ref="N35:R35" si="7">AVERAGE(N32:N34)</f>
+        <v>2.8495772789141753</v>
+      </c>
+      <c r="O35" s="12">
+        <f t="shared" si="7"/>
+        <v>1.8533333333333335</v>
+      </c>
+      <c r="P35" s="12">
+        <f t="shared" si="7"/>
+        <v>1.3298605415632234</v>
+      </c>
+      <c r="Q35" s="12">
+        <f t="shared" si="7"/>
+        <v>2.74598468824E-2</v>
+      </c>
+      <c r="R35" s="12">
+        <f t="shared" si="7"/>
+        <v>2.0014983239344527E-2</v>
       </c>
     </row>
   </sheetData>
@@ -17763,10 +17805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U35" sqref="U35"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35:R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -17791,21 +17833,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
@@ -18871,6 +18913,35 @@
       <c r="R38" s="12">
         <f t="shared" si="5"/>
         <v>1.1604868132979061E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="12:18">
+      <c r="L39" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="M39" s="12">
+        <f>AVERAGE(M36:M38)</f>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="N39" s="12">
+        <f t="shared" ref="N39:R39" si="7">AVERAGE(N36:N38)</f>
+        <v>3.9715420975522462</v>
+      </c>
+      <c r="O39" s="12">
+        <f t="shared" si="7"/>
+        <v>3.2449999999999997</v>
+      </c>
+      <c r="P39" s="12">
+        <f t="shared" si="7"/>
+        <v>2.8135759169278312</v>
+      </c>
+      <c r="Q39" s="12">
+        <f t="shared" si="7"/>
+        <v>2.6645359898599997E-2</v>
+      </c>
+      <c r="R39" s="12">
+        <f t="shared" si="7"/>
+        <v>2.0946195445744335E-2</v>
       </c>
     </row>
   </sheetData>
@@ -18887,8 +18958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19110,8 +19181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK53"/>
   <sheetViews>
-    <sheetView topLeftCell="V13" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="AG20" sqref="AG20"/>
+    <sheetView topLeftCell="V10" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3:AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -19128,6 +19199,11 @@
     <col min="27" max="27" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -19540,32 +19616,59 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
+      <c r="AE10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF10" s="12">
+        <f>AVERAGE(AF4:AF9)</f>
+        <v>32.980284721724487</v>
+      </c>
+      <c r="AG10" s="12">
+        <f t="shared" ref="AG10:AK10" si="0">AVERAGE(AG4:AG9)</f>
+        <v>18.260957317493936</v>
+      </c>
+      <c r="AH10" s="12">
+        <f t="shared" si="0"/>
+        <v>126.36954109659943</v>
+      </c>
+      <c r="AI10" s="12">
+        <f t="shared" si="0"/>
+        <v>8.0733355559358806</v>
+      </c>
+      <c r="AJ10" s="12">
+        <f t="shared" si="0"/>
+        <v>117.6091874897955</v>
+      </c>
+      <c r="AK10" s="12">
+        <f t="shared" si="0"/>
+        <v>15.075808627901134</v>
+      </c>
     </row>
     <row r="11" spans="1:37">
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18" t="s">
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
     </row>
     <row r="12" spans="1:37">
       <c r="D12" s="10" t="s">
@@ -19927,11 +20030,11 @@
         <v>5.0411645755102041E-2</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:F18" si="0">AVERAGE(E13:E17)</f>
+        <f t="shared" ref="E18:F18" si="1">AVERAGE(E13:E17)</f>
         <v>0.14887388379591954</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15096087085714244</v>
       </c>
       <c r="G18">
@@ -19948,11 +20051,11 @@
         <v>2.3060372204081636E-2</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18:L18" si="1">AVERAGE(K13:K17)</f>
+        <f t="shared" ref="K18:L18" si="2">AVERAGE(K13:K17)</f>
         <v>0.12838769693877666</v>
       </c>
       <c r="L18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17323541134693837</v>
       </c>
       <c r="M18">
@@ -20096,30 +20199,30 @@
       <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18" t="s">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18" t="s">
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
     </row>
     <row r="28" spans="1:21">
       <c r="D28" s="10" t="s">
@@ -20481,11 +20584,11 @@
         <v>2.371209908612245E-2</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34" si="2">AVERAGE(E29:E33)</f>
+        <f t="shared" ref="E34" si="3">AVERAGE(E29:E33)</f>
         <v>0.15181541017551142</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34" si="3">AVERAGE(F29:F33)</f>
+        <f t="shared" ref="F34" si="4">AVERAGE(F29:F33)</f>
         <v>0.1175712866857139</v>
       </c>
       <c r="G34">
@@ -20502,11 +20605,11 @@
         <v>2.4355517121775517E-2</v>
       </c>
       <c r="K34">
-        <f t="shared" ref="K34" si="4">AVERAGE(K29:K33)</f>
+        <f t="shared" ref="K34" si="5">AVERAGE(K29:K33)</f>
         <v>0.13865597546530731</v>
       </c>
       <c r="L34">
-        <f t="shared" ref="L34" si="5">AVERAGE(L29:L33)</f>
+        <f t="shared" ref="L34" si="6">AVERAGE(L29:L33)</f>
         <v>4.2796422130611807E-2</v>
       </c>
       <c r="M34">
@@ -20519,15 +20622,15 @@
         <v>1.6371628170412607E-2</v>
       </c>
       <c r="P34">
-        <f t="shared" ref="P34" si="6">AVERAGE(P29:P33)</f>
+        <f t="shared" ref="P34" si="7">AVERAGE(P29:P33)</f>
         <v>3.9156004204081621E-2</v>
       </c>
       <c r="Q34">
-        <f t="shared" ref="Q34" si="7">AVERAGE(Q29:Q33)</f>
+        <f t="shared" ref="Q34" si="8">AVERAGE(Q29:Q33)</f>
         <v>7.2727680816338609E-3</v>
       </c>
       <c r="R34">
-        <f t="shared" ref="R34" si="8">AVERAGE(R29:R33)</f>
+        <f t="shared" ref="R34" si="9">AVERAGE(R29:R33)</f>
         <v>0.10524139840816285</v>
       </c>
       <c r="S34">
@@ -20784,23 +20887,23 @@
         <v>50.411645755102043</v>
       </c>
       <c r="E43" s="12">
-        <f t="shared" ref="E43:I43" si="9">E38*1000</f>
+        <f t="shared" ref="E43:I43" si="10">E38*1000</f>
         <v>22.812616890718406</v>
       </c>
       <c r="F43" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>148.87388379591954</v>
       </c>
       <c r="G43" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.329816685869007</v>
       </c>
       <c r="H43" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>150.96087085714242</v>
       </c>
       <c r="I43" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.613304472821564</v>
       </c>
       <c r="J43" s="4"/>
@@ -20812,23 +20915,23 @@
         <v>23.71209908612245</v>
       </c>
       <c r="M43" s="12">
-        <f t="shared" ref="M43:Q43" si="10">M38*1000</f>
+        <f t="shared" ref="M43:Q43" si="11">M38*1000</f>
         <v>16.059335823724702</v>
       </c>
       <c r="N43" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>151.81541017551143</v>
       </c>
       <c r="O43" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.8562847757825898</v>
       </c>
       <c r="P43" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>117.5712866857139</v>
       </c>
       <c r="Q43" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12.807851760857263</v>
       </c>
     </row>
@@ -20837,27 +20940,27 @@
         <v>17</v>
       </c>
       <c r="D44" s="12">
-        <f t="shared" ref="D44:I44" si="11">D39*1000</f>
+        <f t="shared" ref="D44:I44" si="12">D39*1000</f>
         <v>23.060372204081638</v>
       </c>
       <c r="E44" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14.85094483747665</v>
       </c>
       <c r="F44" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>128.38769693877666</v>
       </c>
       <c r="G44" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.482378513474547</v>
       </c>
       <c r="H44" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>173.23541134693838</v>
       </c>
       <c r="I44" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>23.235821145735382</v>
       </c>
       <c r="J44" s="4"/>
@@ -20865,27 +20968,27 @@
         <v>17</v>
       </c>
       <c r="L44" s="12">
-        <f t="shared" ref="L44:Q44" si="12">L39*1000</f>
+        <f t="shared" ref="L44:Q44" si="13">L39*1000</f>
         <v>24.355517121775517</v>
       </c>
       <c r="M44" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17.472085512364</v>
       </c>
       <c r="N44" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>138.65597546530731</v>
       </c>
       <c r="O44" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.772731672518213</v>
       </c>
       <c r="P44" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>42.796422130611809</v>
       </c>
       <c r="Q44" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>16.371628170412606</v>
       </c>
     </row>
@@ -20894,27 +20997,27 @@
         <v>18</v>
       </c>
       <c r="D45" s="12">
-        <f t="shared" ref="D45:I45" si="13">D40*1000</f>
+        <f t="shared" ref="D45:I45" si="14">D40*1000</f>
         <v>37.186069959183662</v>
       </c>
       <c r="E45" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14.850241997686163</v>
       </c>
       <c r="F45" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>183.2115121224478</v>
       </c>
       <c r="G45" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7.296972233069174</v>
       </c>
       <c r="H45" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>115.84973551020366</v>
       </c>
       <c r="I45" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16.265329219752218</v>
       </c>
       <c r="J45" s="4"/>
@@ -20922,27 +21025,27 @@
         <v>18</v>
       </c>
       <c r="L45" s="12">
-        <f t="shared" ref="L45:Q45" si="14">L40*1000</f>
+        <f t="shared" ref="L45:Q45" si="15">L40*1000</f>
         <v>39.156004204081619</v>
       </c>
       <c r="M45" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23.520518842993702</v>
       </c>
       <c r="N45" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.2727680816338607</v>
       </c>
       <c r="O45" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.7018294549017585</v>
       </c>
       <c r="P45" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>105.24139840816285</v>
       </c>
       <c r="Q45" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.1609169978277656</v>
       </c>
     </row>
@@ -34837,8 +34940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4:AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -34846,12 +34949,12 @@
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -35023,6 +35126,33 @@
       <c r="H8" t="s">
         <v>16</v>
       </c>
+      <c r="W8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="X8" s="15">
+        <f>AVERAGE(X5:X7)</f>
+        <v>87.499831319727903</v>
+      </c>
+      <c r="Y8" s="15">
+        <f t="shared" ref="Y8:AC8" si="0">AVERAGE(Y5:Y7)</f>
+        <v>37.23707457109218</v>
+      </c>
+      <c r="Z8" s="15">
+        <f t="shared" si="0"/>
+        <v>30.220642680272491</v>
+      </c>
+      <c r="AA8" s="15">
+        <f t="shared" si="0"/>
+        <v>5.5938400446366385</v>
+      </c>
+      <c r="AB8" s="15">
+        <f t="shared" si="0"/>
+        <v>55.104023142857557</v>
+      </c>
+      <c r="AC8" s="15">
+        <f t="shared" si="0"/>
+        <v>7.8426592784375861</v>
+      </c>
     </row>
     <row r="10" spans="1:29">
       <c r="D10" s="9" t="s">
@@ -35030,30 +35160,30 @@
       </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18" t="s">
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
     </row>
     <row r="12" spans="1:29">
       <c r="D12" s="10" t="s">
@@ -35436,11 +35566,11 @@
         <v>0.16385187742857152</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18:L18" si="0">AVERAGE(K13:K17)</f>
+        <f t="shared" ref="K18:L18" si="1">AVERAGE(K13:K17)</f>
         <v>3.631794167347057E-2</v>
       </c>
       <c r="L18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5307936734694253E-2</v>
       </c>
       <c r="M18">
@@ -35592,23 +35722,23 @@
         <v>14.321220326530609</v>
       </c>
       <c r="E26" s="12">
-        <f t="shared" ref="E26:I26" si="1">E21*1000</f>
+        <f t="shared" ref="E26:I26" si="2">E21*1000</f>
         <v>9.7528125996814889</v>
       </c>
       <c r="F26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0354551428582948</v>
       </c>
       <c r="G26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6514173157597045</v>
       </c>
       <c r="H26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84.768485061224908</v>
       </c>
       <c r="I26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4998927479912481</v>
       </c>
     </row>
@@ -35617,27 +35747,27 @@
         <v>2</v>
       </c>
       <c r="D27" s="12">
-        <f t="shared" ref="D27:I27" si="2">D22*1000</f>
+        <f t="shared" ref="D27:I27" si="3">D22*1000</f>
         <v>163.85187742857153</v>
       </c>
       <c r="E27" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57.584815382371353</v>
       </c>
       <c r="F27" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36.317941673470571</v>
       </c>
       <c r="G27" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.6522160335718805</v>
       </c>
       <c r="H27" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25.307936734694252</v>
       </c>
       <c r="I27" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.457090225613635</v>
       </c>
     </row>
@@ -35646,27 +35776,27 @@
         <v>3</v>
       </c>
       <c r="D28" s="12">
-        <f t="shared" ref="D28:I28" si="3">D23*1000</f>
+        <f t="shared" ref="D28:I28" si="4">D23*1000</f>
         <v>84.326396204081604</v>
       </c>
       <c r="E28" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44.373595731223702</v>
       </c>
       <c r="F28" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50.308531224488604</v>
       </c>
       <c r="G28" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.4778867845783301</v>
       </c>
       <c r="H28" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55.235647632653496</v>
       </c>
       <c r="I28" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5709948617078737</v>
       </c>
     </row>
@@ -42852,10 +42982,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AE30"/>
+  <dimension ref="B2:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Z7"/>
+    <sheetView tabSelected="1" topLeftCell="Q22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="X32" sqref="X32:AD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -43555,7 +43685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:30">
       <c r="C18" t="s">
         <v>38</v>
       </c>
@@ -43575,7 +43705,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:30">
       <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
@@ -43600,7 +43730,7 @@
         <v>0.55528034791219627</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:30">
       <c r="B20" s="8" t="s">
         <v>34</v>
       </c>
@@ -43625,7 +43755,7 @@
         <v>0.4624551752617776</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:30">
       <c r="B21" s="8" t="s">
         <v>36</v>
       </c>
@@ -43650,7 +43780,7 @@
         <v>0.69631842561330615</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:30">
       <c r="B22" s="8" t="s">
         <v>37</v>
       </c>
@@ -43673,7 +43803,7 @@
         <v>1.3841407208010446</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:30">
       <c r="B23" s="14" t="s">
         <v>7</v>
       </c>
@@ -43698,10 +43828,10 @@
         <v>3.7531144658241318</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:30">
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:30">
       <c r="C25" t="s">
         <v>38</v>
       </c>
@@ -43721,7 +43851,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:30">
       <c r="B26" s="14" t="s">
         <v>44</v>
       </c>
@@ -43750,7 +43880,7 @@
         <v>0.71061691307878794</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:30">
       <c r="B27" s="14" t="s">
         <v>45</v>
       </c>
@@ -43779,7 +43909,7 @@
         <v>0.9130975157014134</v>
       </c>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:30">
       <c r="B28" s="14" t="s">
         <v>46</v>
       </c>
@@ -43808,7 +43938,7 @@
         <v>0.32312334800954079</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:30">
       <c r="B29" s="14" t="s">
         <v>47</v>
       </c>
@@ -43837,7 +43967,7 @@
         <v>0.40020607912455636</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:30">
       <c r="B30" s="14" t="s">
         <v>7</v>
       </c>
@@ -43864,6 +43994,280 @@
       <c r="H30">
         <f>L15</f>
         <v>2.8849065320762284</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30">
+      <c r="Q32" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="R32" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="S32" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="T32" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="U32" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="V32" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z32" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA32" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB32" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC32" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD32" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="16:31">
+      <c r="P33" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q33" s="15">
+        <v>1.4379256874499888</v>
+      </c>
+      <c r="R33" s="15">
+        <v>1.2452117860740748</v>
+      </c>
+      <c r="S33" s="15">
+        <v>0.7004587177831999</v>
+      </c>
+      <c r="T33" s="15">
+        <v>0.42779289942026016</v>
+      </c>
+      <c r="U33" s="15">
+        <v>0.8226217746508</v>
+      </c>
+      <c r="V33" s="15">
+        <v>0.55528034791219627</v>
+      </c>
+      <c r="X33" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y33" s="15">
+        <v>2.3394612909499926</v>
+      </c>
+      <c r="Z33" s="15">
+        <v>1.2905525335294337</v>
+      </c>
+      <c r="AA33" s="15">
+        <v>1.4623187491849496</v>
+      </c>
+      <c r="AB33" s="15">
+        <v>0.20569798692045349</v>
+      </c>
+      <c r="AC33" s="15">
+        <v>1.1723496824234998</v>
+      </c>
+      <c r="AD33" s="15">
+        <v>0.71061691307878794</v>
+      </c>
+      <c r="AE33" s="15"/>
+    </row>
+    <row r="34" spans="16:31">
+      <c r="P34" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q34" s="15">
+        <v>1.8904397705199898</v>
+      </c>
+      <c r="R34" s="15">
+        <v>1.5553417988587652</v>
+      </c>
+      <c r="S34" s="15">
+        <v>0.6610034153655</v>
+      </c>
+      <c r="T34" s="15">
+        <v>0.38951274739045838</v>
+      </c>
+      <c r="U34" s="15">
+        <v>1.8863402021275</v>
+      </c>
+      <c r="V34" s="15">
+        <v>0.4624551752617776</v>
+      </c>
+      <c r="X34" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y34" s="15">
+        <v>1.6025620354100241</v>
+      </c>
+      <c r="Z34" s="15">
+        <v>2.2193070676137543</v>
+      </c>
+      <c r="AA34" s="15">
+        <v>1.2712261936695</v>
+      </c>
+      <c r="AB34" s="15">
+        <v>0.21773132733639453</v>
+      </c>
+      <c r="AC34" s="15">
+        <v>1.4809864287569001</v>
+      </c>
+      <c r="AD34" s="15">
+        <v>0.9130975157014134</v>
+      </c>
+      <c r="AE34" s="15"/>
+    </row>
+    <row r="35" spans="16:31">
+      <c r="P35" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q35" s="15">
+        <v>2.1545246432799927</v>
+      </c>
+      <c r="R35" s="15">
+        <v>1.8262796506149472</v>
+      </c>
+      <c r="S35" s="15">
+        <v>0.53135775189925016</v>
+      </c>
+      <c r="T35" s="15">
+        <v>0.3041001456456614</v>
+      </c>
+      <c r="U35" s="15">
+        <v>4.0568488973765007</v>
+      </c>
+      <c r="V35" s="15">
+        <v>0.69631842561330615</v>
+      </c>
+      <c r="X35" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y35" s="15">
+        <v>4.3849408243599983</v>
+      </c>
+      <c r="Z35" s="15">
+        <v>2.4603622093955124</v>
+      </c>
+      <c r="AA35" s="15">
+        <v>0.77643865897499953</v>
+      </c>
+      <c r="AB35" s="15">
+        <v>0.34194728385708173</v>
+      </c>
+      <c r="AC35" s="15">
+        <v>3.8070138477485003</v>
+      </c>
+      <c r="AD35" s="15">
+        <v>0.32312334800954079</v>
+      </c>
+      <c r="AE35" s="15"/>
+    </row>
+    <row r="36" spans="16:31">
+      <c r="P36" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36" s="15">
+        <v>2.7089384818500095</v>
+      </c>
+      <c r="R36" s="15">
+        <v>2.7089384818500095</v>
+      </c>
+      <c r="S36" s="15">
+        <v>0.30866924089999948</v>
+      </c>
+      <c r="T36" s="15">
+        <v>0.21153583906201062</v>
+      </c>
+      <c r="U36" s="15">
+        <v>10.254127724689999</v>
+      </c>
+      <c r="V36" s="15">
+        <v>1.3841407208010446</v>
+      </c>
+      <c r="X36" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y36" s="15">
+        <v>3.3181921509000007</v>
+      </c>
+      <c r="Z36" s="15">
+        <v>1.9487186388892102</v>
+      </c>
+      <c r="AA36" s="15">
+        <v>0.79282525708999929</v>
+      </c>
+      <c r="AB36" s="15">
+        <v>0.59831355441738954</v>
+      </c>
+      <c r="AC36" s="15">
+        <v>8.2129777165049997</v>
+      </c>
+      <c r="AD36" s="15">
+        <v>0.40020607912455636</v>
+      </c>
+      <c r="AE36" s="15"/>
+    </row>
+    <row r="37" spans="16:31">
+      <c r="P37" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q37" s="15">
+        <v>2.047957145774995</v>
+      </c>
+      <c r="R37" s="15">
+        <f>AVERAGE(R33:R36)</f>
+        <v>1.8339429293494491</v>
+      </c>
+      <c r="S37" s="15">
+        <f t="shared" ref="S37:V37" si="0">AVERAGE(S33:S36)</f>
+        <v>0.55037228148698747</v>
+      </c>
+      <c r="T37" s="15">
+        <f t="shared" si="0"/>
+        <v>0.3332354078795976</v>
+      </c>
+      <c r="U37" s="15">
+        <f t="shared" si="0"/>
+        <v>4.2549846497111998</v>
+      </c>
+      <c r="V37" s="15">
+        <f t="shared" si="0"/>
+        <v>0.77454866739708117</v>
+      </c>
+      <c r="X37" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y37" s="15">
+        <f>AVERAGE(Y33:Y36)</f>
+        <v>2.911289075405004</v>
+      </c>
+      <c r="Z37" s="15">
+        <f t="shared" ref="Z37:AD37" si="1">AVERAGE(Z33:Z36)</f>
+        <v>1.9797351123569777</v>
+      </c>
+      <c r="AA37" s="15">
+        <f t="shared" si="1"/>
+        <v>1.0757022147298623</v>
+      </c>
+      <c r="AB37" s="15">
+        <f t="shared" si="1"/>
+        <v>0.3409225381328298</v>
+      </c>
+      <c r="AC37" s="15">
+        <f t="shared" si="1"/>
+        <v>3.6683319188584749</v>
+      </c>
+      <c r="AD37" s="15">
+        <f t="shared" si="1"/>
+        <v>0.58676096397857458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated primesense ar_tag fig, updated 5.3, and finished chapter 5
</commit_message>
<xml_diff>
--- a/tables/final_compiled_test_results_and_figs.xlsx
+++ b/tables/final_compiled_test_results_and_figs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="8145" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="8145" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Fetch_Nav" sheetId="1" r:id="rId1"/>
@@ -352,13 +352,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1142,11 +1142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-229806880"/>
-        <c:axId val="-229816128"/>
+        <c:axId val="1042457680"/>
+        <c:axId val="1042456592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-229806880"/>
+        <c:axId val="1042457680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -1284,12 +1284,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229816128"/>
+        <c:crossAx val="1042456592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-229816128"/>
+        <c:axId val="1042456592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -1427,7 +1427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229806880"/>
+        <c:crossAx val="1042457680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2266,11 +2266,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-229813952"/>
-        <c:axId val="-229809056"/>
+        <c:axId val="1042459312"/>
+        <c:axId val="1042464752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-229813952"/>
+        <c:axId val="1042459312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -2405,12 +2405,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229809056"/>
+        <c:crossAx val="1042464752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-229809056"/>
+        <c:axId val="1042464752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -2539,7 +2539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229813952"/>
+        <c:crossAx val="1042459312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3019,11 +3019,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-229817216"/>
-        <c:axId val="-229803072"/>
+        <c:axId val="1042461488"/>
+        <c:axId val="938065344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-229817216"/>
+        <c:axId val="1042461488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -3158,12 +3158,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229803072"/>
+        <c:crossAx val="938065344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-229803072"/>
+        <c:axId val="938065344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -3292,7 +3292,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229817216"/>
+        <c:crossAx val="1042461488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3760,11 +3760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-229815584"/>
-        <c:axId val="-229814496"/>
+        <c:axId val="938061536"/>
+        <c:axId val="938068608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-229815584"/>
+        <c:axId val="938061536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21"/>
@@ -3893,12 +3893,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229814496"/>
+        <c:crossAx val="938068608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-229814496"/>
+        <c:axId val="938068608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -4027,7 +4027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229815584"/>
+        <c:crossAx val="938061536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4216,10 +4216,10 @@
                   <c:v>23.060372204081638</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.186069959183662</c:v>
+                  <c:v>24.355517121775517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.355517121775517</c:v>
+                  <c:v>37.186069959183662</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>39.156004204081619</c:v>
@@ -4310,10 +4310,10 @@
                   <c:v>128.38769693877666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>183.2115121224478</c:v>
+                  <c:v>138.65597546530731</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>138.65597546530731</c:v>
+                  <c:v>183.2115121224478</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7.2727680816338607</c:v>
@@ -4404,10 +4404,10 @@
                   <c:v>173.23541134693838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>115.84973551020366</c:v>
+                  <c:v>42.796422130611809</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.796422130611809</c:v>
+                  <c:v>115.84973551020366</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>105.24139840816285</c:v>
@@ -4790,7 +4790,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>37.186069959183662</c:v>
+                  <c:v>24.355517121775517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4885,7 +4885,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24.355517121775517</c:v>
+                  <c:v>37.186069959183662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5360,7 +5360,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>183.2115121224478</c:v>
+                  <c:v>138.65597546530731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5455,7 +5455,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>138.65597546530731</c:v>
+                  <c:v>183.2115121224478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5930,7 +5930,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>115.84973551020366</c:v>
+                  <c:v>42.796422130611809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6025,7 +6025,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>42.796422130611809</c:v>
+                  <c:v>115.84973551020366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6135,11 +6135,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-231330304"/>
-        <c:axId val="-84761952"/>
+        <c:axId val="938063712"/>
+        <c:axId val="938072416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-231330304"/>
+        <c:axId val="938063712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7"/>
@@ -6268,12 +6268,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84761952"/>
+        <c:crossAx val="938072416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-84761952"/>
+        <c:axId val="938072416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -6410,7 +6410,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-231330304"/>
+        <c:crossAx val="938063712"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7669,11 +7669,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-84761408"/>
-        <c:axId val="-84755968"/>
+        <c:axId val="938060448"/>
+        <c:axId val="938069152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-84761408"/>
+        <c:axId val="938060448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -7802,12 +7802,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84755968"/>
+        <c:crossAx val="938069152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-84755968"/>
+        <c:axId val="938069152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="225"/>
@@ -7945,7 +7945,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84761408"/>
+        <c:crossAx val="938060448"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -9472,11 +9472,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-84754880"/>
-        <c:axId val="-84760864"/>
+        <c:axId val="938068064"/>
+        <c:axId val="938069696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-84754880"/>
+        <c:axId val="938068064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -9605,12 +9605,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84760864"/>
+        <c:crossAx val="938069696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-84760864"/>
+        <c:axId val="938069696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18"/>
@@ -9748,7 +9748,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84754880"/>
+        <c:crossAx val="938068064"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11286,11 +11286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-84759232"/>
-        <c:axId val="-84758688"/>
+        <c:axId val="938067520"/>
+        <c:axId val="938060992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-84759232"/>
+        <c:axId val="938067520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -11419,12 +11419,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84758688"/>
+        <c:crossAx val="938060992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-84758688"/>
+        <c:axId val="938060992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -11562,7 +11562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84759232"/>
+        <c:crossAx val="938067520"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16269,16 +16269,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>122705</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>124663</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>555624</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>124199</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>10363</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16667,7 +16667,1147 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31:R35"/>
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="G3" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>10.4</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="6">
+        <f>7-5.1</f>
+        <v>1.9000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G4" s="6">
+        <v>9.9999999999999603E-2</v>
+      </c>
+      <c r="H4" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="J4" s="6">
+        <f>7-5.7</f>
+        <v>1.2999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>11.9</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="H5" s="6">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="J5" s="6">
+        <f>7-5.3</f>
+        <v>1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="D6" s="6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="6">
+        <v>6.8</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="H6" s="6">
+        <v>8.9</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="6">
+        <f>8.2-7</f>
+        <v>1.1999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9.9999999999999603E-2</v>
+      </c>
+      <c r="H7" s="6">
+        <v>6.3</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="J7" s="6">
+        <f>7.1-7</f>
+        <v>9.9999999999999645E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="F8" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="G8" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="H8" s="6">
+        <v>5.7</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <f>7-6.6</f>
+        <v>0.40000000000000036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>7</v>
+      </c>
+      <c r="F9" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H9" s="6">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="6">
+        <f>9.3-7</f>
+        <v>2.3000000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="H10" s="6">
+        <v>7.1</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="J10" s="6">
+        <f>8-7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="H11" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="I11" s="6">
+        <v>3.4</v>
+      </c>
+      <c r="J11" s="6">
+        <f>7-5.8</f>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C12" s="6">
+        <v>3.4</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E12" s="6">
+        <v>5.8</v>
+      </c>
+      <c r="F12" s="6">
+        <v>6.6</v>
+      </c>
+      <c r="G12" s="6">
+        <v>9.9999999999999603E-2</v>
+      </c>
+      <c r="H12" s="6">
+        <v>6.2</v>
+      </c>
+      <c r="I12" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="J12" s="6">
+        <f>7-6.1</f>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="H13" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="I13" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="J13" s="6">
+        <f>5.1-2.2</f>
+        <v>2.8999999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
+        <v>6.1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="D14" s="6">
+        <v>9.9999999999999603E-2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="J14" s="6">
+        <f>4.2-2.2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6">
+        <v>10.3</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F15" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="G15" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="H15" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="J15" s="6">
+        <f>5.4-2.2</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="G16" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="I16" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="J16" s="6">
+        <f>5.6-2.2</f>
+        <v>3.3999999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6">
+        <v>5.9</v>
+      </c>
+      <c r="I17" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="J17" s="6">
+        <f>5.1-2.2</f>
+        <v>2.8999999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6">
+        <v>7.8</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="H18" s="6">
+        <v>6.1</v>
+      </c>
+      <c r="I18" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="J18" s="6">
+        <f>2.2-2.1</f>
+        <v>0.10000000000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="E19" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="H19" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="J19" s="6">
+        <f>4.7-2.2</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6">
+        <v>6.1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="H20" s="6">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I20" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="J20" s="6">
+        <f>2.2-2.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E21" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="F21" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="G21" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I21" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="J21" s="6">
+        <f>2.2-2.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6">
+        <v>2</v>
+      </c>
+      <c r="E22" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="G22" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I22" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="J22" s="6">
+        <f>2.4-2.2</f>
+        <v>0.19999999999999973</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="6">
+        <f>AVERAGE((B3:B22))</f>
+        <v>4.25</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" ref="C24:J24" si="0">AVERAGE((C3:C22))</f>
+        <v>1.4749999999999999</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5650000000000002</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="0"/>
+        <v>3.9249999999999994</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5649999999999999</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6949999999999998</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="0"/>
+        <v>5.82</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="0"/>
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="6">
+        <f>STDEV(B3:B22)</f>
+        <v>2.5037866060071998</v>
+      </c>
+      <c r="C25" s="6">
+        <f>STDEV(C3:C22)</f>
+        <v>1.2268380410418354</v>
+      </c>
+      <c r="D25" s="6">
+        <f>STDEV(D3:D22)</f>
+        <v>1.053452968999915</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" ref="E25:J25" si="1">STDEV(E3:E22)</f>
+        <v>2.6183311277867145</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6560177344588152</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2483568147136885</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" si="1"/>
+        <v>3.4266141029486121</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="1"/>
+        <v>1.10672584918902</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="1"/>
+        <v>1.1385124181649446</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="6">
+        <f>B24+B25*3</f>
+        <v>11.761359818021599</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" ref="C26:J26" si="2">C24+C25*3</f>
+        <v>5.1555141231255055</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="2"/>
+        <v>4.7253589069997455</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="2"/>
+        <v>11.779993383360143</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="2"/>
+        <v>7.5330532033764452</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4400704441410657</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="2"/>
+        <v>16.099842308845837</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="2"/>
+        <v>4.8401775475670599</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="2"/>
+        <v>4.8755372544948337</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N26" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="O26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="P26" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R26" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="U26" s="3"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M27" s="12">
+        <v>4.25</v>
+      </c>
+      <c r="N27" s="12">
+        <v>2.5037866060071998</v>
+      </c>
+      <c r="O27" s="12">
+        <v>1.4749999999999999</v>
+      </c>
+      <c r="P27" s="12">
+        <v>1.2268380410418354</v>
+      </c>
+      <c r="Q27" s="12">
+        <v>1.5650000000000002</v>
+      </c>
+      <c r="R27" s="12">
+        <v>1.053452968999915</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M28" s="12">
+        <v>3.9249999999999994</v>
+      </c>
+      <c r="N28" s="12">
+        <v>2.6183311277867145</v>
+      </c>
+      <c r="O28" s="12">
+        <v>2.5649999999999999</v>
+      </c>
+      <c r="P28" s="12">
+        <v>1.6560177344588152</v>
+      </c>
+      <c r="Q28" s="12">
+        <v>1.6949999999999998</v>
+      </c>
+      <c r="R28" s="12">
+        <v>1.2483568147136885</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="B29" s="6">
+        <f>MAX(B26,E26,H26)</f>
+        <v>16.099842308845837</v>
+      </c>
+      <c r="C29" s="6">
+        <f>MAX(C26,F26,I26)</f>
+        <v>7.5330532033764452</v>
+      </c>
+      <c r="D29" s="6">
+        <f>MAX(D26,G26,J26)</f>
+        <v>5.4400704441410657</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M29" s="12">
+        <v>5.82</v>
+      </c>
+      <c r="N29" s="12">
+        <v>3.4266141029486121</v>
+      </c>
+      <c r="O29" s="12">
+        <v>1.52</v>
+      </c>
+      <c r="P29" s="12">
+        <v>1.10672584918902</v>
+      </c>
+      <c r="Q29" s="12">
+        <v>1.46</v>
+      </c>
+      <c r="R29" s="12">
+        <v>1.1385124181649446</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="M31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="O31" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="P31" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="R31" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="E32" s="6"/>
+      <c r="L32" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M32" s="12">
+        <f>M27</f>
+        <v>4.25</v>
+      </c>
+      <c r="N32" s="12">
+        <f t="shared" ref="N32:P32" si="3">N27</f>
+        <v>2.5037866060071998</v>
+      </c>
+      <c r="O32" s="12">
+        <f t="shared" si="3"/>
+        <v>1.4749999999999999</v>
+      </c>
+      <c r="P32" s="12">
+        <f t="shared" si="3"/>
+        <v>1.2268380410418354</v>
+      </c>
+      <c r="Q32" s="12">
+        <f t="shared" ref="Q32:R34" si="4">Q27*0.01745329251</f>
+        <v>2.7314402778150001E-2</v>
+      </c>
+      <c r="R32" s="12">
+        <f t="shared" si="4"/>
+        <v>1.8386222813483479E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="12:18">
+      <c r="L33" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M33" s="12">
+        <f t="shared" ref="M33:P33" si="5">M28</f>
+        <v>3.9249999999999994</v>
+      </c>
+      <c r="N33" s="12">
+        <f t="shared" si="5"/>
+        <v>2.6183311277867145</v>
+      </c>
+      <c r="O33" s="12">
+        <f t="shared" si="5"/>
+        <v>2.5649999999999999</v>
+      </c>
+      <c r="P33" s="12">
+        <f t="shared" si="5"/>
+        <v>1.6560177344588152</v>
+      </c>
+      <c r="Q33" s="12">
+        <f t="shared" si="4"/>
+        <v>2.9583330804449998E-2</v>
+      </c>
+      <c r="R33" s="12">
+        <f t="shared" si="4"/>
+        <v>2.1787936644049877E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="12:18">
+      <c r="L34" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M34" s="12">
+        <f t="shared" ref="M34:P34" si="6">M29</f>
+        <v>5.82</v>
+      </c>
+      <c r="N34" s="12">
+        <f t="shared" si="6"/>
+        <v>3.4266141029486121</v>
+      </c>
+      <c r="O34" s="12">
+        <f t="shared" si="6"/>
+        <v>1.52</v>
+      </c>
+      <c r="P34" s="12">
+        <f t="shared" si="6"/>
+        <v>1.10672584918902</v>
+      </c>
+      <c r="Q34" s="12">
+        <f t="shared" si="4"/>
+        <v>2.5481807064599998E-2</v>
+      </c>
+      <c r="R34" s="12">
+        <f t="shared" si="4"/>
+        <v>1.9870790260500214E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="12:18">
+      <c r="L35" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="12">
+        <f>AVERAGE(M32:M34)</f>
+        <v>4.665</v>
+      </c>
+      <c r="N35" s="12">
+        <f t="shared" ref="N35:R35" si="7">AVERAGE(N32:N34)</f>
+        <v>2.8495772789141753</v>
+      </c>
+      <c r="O35" s="12">
+        <f t="shared" si="7"/>
+        <v>1.8533333333333335</v>
+      </c>
+      <c r="P35" s="12">
+        <f t="shared" si="7"/>
+        <v>1.3298605415632234</v>
+      </c>
+      <c r="Q35" s="12">
+        <f t="shared" si="7"/>
+        <v>2.74598468824E-2</v>
+      </c>
+      <c r="R35" s="12">
+        <f t="shared" si="7"/>
+        <v>2.0014983239344527E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -16692,1162 +17832,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="D3" s="6">
-        <v>3</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1.6</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1.8</v>
-      </c>
-      <c r="G3" s="6">
-        <v>3.1</v>
-      </c>
-      <c r="H3" s="6">
-        <v>10.4</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="6">
-        <f>7-5.1</f>
-        <v>1.9000000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1.7</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="E4" s="6">
-        <v>3.6</v>
-      </c>
-      <c r="F4" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G4" s="6">
-        <v>9.9999999999999603E-2</v>
-      </c>
-      <c r="H4" s="6">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="J4" s="6">
-        <f>7-5.7</f>
-        <v>1.2999999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6">
-        <v>2.1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1.3</v>
-      </c>
-      <c r="D5" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="E5" s="6">
-        <v>11.9</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G5" s="6">
-        <v>3.7</v>
-      </c>
-      <c r="H5" s="6">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="J5" s="6">
-        <f>7-5.3</f>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1.6</v>
-      </c>
-      <c r="D6" s="6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="6">
-        <v>6.8</v>
-      </c>
-      <c r="F6" s="6">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G6" s="6">
-        <v>2.7</v>
-      </c>
-      <c r="H6" s="6">
-        <v>8.9</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J6" s="6">
-        <f>8.2-7</f>
-        <v>1.1999999999999993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="D7" s="6">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1.8</v>
-      </c>
-      <c r="F7" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="G7" s="6">
-        <v>9.9999999999999603E-2</v>
-      </c>
-      <c r="H7" s="6">
-        <v>6.3</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="J7" s="6">
-        <f>7.1-7</f>
-        <v>9.9999999999999645E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6">
-        <v>3.9</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1.9</v>
-      </c>
-      <c r="E8" s="6">
-        <v>3.9</v>
-      </c>
-      <c r="F8" s="6">
-        <v>2.9</v>
-      </c>
-      <c r="G8" s="6">
-        <v>3.3</v>
-      </c>
-      <c r="H8" s="6">
-        <v>5.7</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <f>7-6.6</f>
-        <v>0.40000000000000036</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1.7</v>
-      </c>
-      <c r="D9" s="6">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6">
-        <v>7</v>
-      </c>
-      <c r="F9" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H9" s="6">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J9" s="6">
-        <f>9.3-7</f>
-        <v>2.3000000000000007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="C10" s="6">
-        <v>3</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="F10" s="6">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="H10" s="6">
-        <v>7.1</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1.7</v>
-      </c>
-      <c r="J10" s="6">
-        <f>8-7</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6">
-        <v>6.5</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6">
-        <v>4.3</v>
-      </c>
-      <c r="F11" s="6">
-        <v>5</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="H11" s="6">
-        <v>12.5</v>
-      </c>
-      <c r="I11" s="6">
-        <v>3.4</v>
-      </c>
-      <c r="J11" s="6">
-        <f>7-5.8</f>
-        <v>1.2000000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="C12" s="6">
-        <v>3.4</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="E12" s="6">
-        <v>5.8</v>
-      </c>
-      <c r="F12" s="6">
-        <v>6.6</v>
-      </c>
-      <c r="G12" s="6">
-        <v>9.9999999999999603E-2</v>
-      </c>
-      <c r="H12" s="6">
-        <v>6.2</v>
-      </c>
-      <c r="I12" s="6">
-        <v>2.1</v>
-      </c>
-      <c r="J12" s="6">
-        <f>7-6.1</f>
-        <v>0.90000000000000036</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="6">
-        <v>8</v>
-      </c>
-      <c r="C13" s="6">
-        <v>2.1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>2</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6">
-        <v>2.8</v>
-      </c>
-      <c r="H13" s="6">
-        <v>3.7</v>
-      </c>
-      <c r="I13" s="6">
-        <v>2.8</v>
-      </c>
-      <c r="J13" s="6">
-        <f>5.1-2.2</f>
-        <v>2.8999999999999995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="6">
-        <v>6.1</v>
-      </c>
-      <c r="C14" s="6">
-        <v>4.8</v>
-      </c>
-      <c r="D14" s="6">
-        <v>9.9999999999999603E-2</v>
-      </c>
-      <c r="E14" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="F14" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="G14" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H14" s="6">
-        <v>1</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="J14" s="6">
-        <f>4.2-2.2</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6">
-        <v>10.3</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="D15" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="E15" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F15" s="6">
-        <v>3.9</v>
-      </c>
-      <c r="G15" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="H15" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="J15" s="6">
-        <f>5.4-2.2</f>
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6">
-        <v>3.5</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="D16" s="6">
-        <v>2</v>
-      </c>
-      <c r="E16" s="6">
-        <v>3.8</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1.9</v>
-      </c>
-      <c r="G16" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="H16" s="6">
-        <v>1.9</v>
-      </c>
-      <c r="I16" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="J16" s="6">
-        <f>5.6-2.2</f>
-        <v>3.3999999999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="6">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="6">
-        <v>3.2</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1.7</v>
-      </c>
-      <c r="G17" s="6">
-        <v>1</v>
-      </c>
-      <c r="H17" s="6">
-        <v>5.9</v>
-      </c>
-      <c r="I17" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="J17" s="6">
-        <f>5.1-2.2</f>
-        <v>2.8999999999999995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6">
-        <v>7.8</v>
-      </c>
-      <c r="C18" s="6">
-        <v>1.4</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="F18" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="G18" s="6">
-        <v>1.3</v>
-      </c>
-      <c r="H18" s="6">
-        <v>6.1</v>
-      </c>
-      <c r="I18" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="J18" s="6">
-        <f>2.2-2.1</f>
-        <v>0.10000000000000009</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6">
-        <v>4</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1.4</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="E19" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1.9</v>
-      </c>
-      <c r="G19" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="H19" s="6">
-        <v>2.7</v>
-      </c>
-      <c r="I19" s="6">
-        <v>1.9</v>
-      </c>
-      <c r="J19" s="6">
-        <f>4.7-2.2</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="6">
-        <v>6.1</v>
-      </c>
-      <c r="C20" s="6">
-        <v>2</v>
-      </c>
-      <c r="D20" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F20" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="G20" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="H20" s="6">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I20" s="6">
-        <v>3.5</v>
-      </c>
-      <c r="J20" s="6">
-        <f>2.2-2.2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="E21" s="6">
-        <v>5.5</v>
-      </c>
-      <c r="F21" s="6">
-        <v>2.6</v>
-      </c>
-      <c r="G21" s="6">
-        <v>3.5</v>
-      </c>
-      <c r="H21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I21" s="6">
-        <v>1.9</v>
-      </c>
-      <c r="J21" s="6">
-        <f>2.2-2.2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" s="6">
-        <v>3.3</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6">
-        <v>2</v>
-      </c>
-      <c r="E22" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F22" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="G22" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="I22" s="6">
-        <v>1.4</v>
-      </c>
-      <c r="J22" s="6">
-        <f>2.4-2.2</f>
-        <v>0.19999999999999973</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:21">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="6">
-        <f>AVERAGE((B3:B22))</f>
-        <v>4.25</v>
-      </c>
-      <c r="C24" s="6">
-        <f t="shared" ref="C24:J24" si="0">AVERAGE((C3:C22))</f>
-        <v>1.4749999999999999</v>
-      </c>
-      <c r="D24" s="6">
-        <f t="shared" si="0"/>
-        <v>1.5650000000000002</v>
-      </c>
-      <c r="E24" s="6">
-        <f t="shared" si="0"/>
-        <v>3.9249999999999994</v>
-      </c>
-      <c r="F24" s="6">
-        <f t="shared" si="0"/>
-        <v>2.5649999999999999</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="0"/>
-        <v>1.6949999999999998</v>
-      </c>
-      <c r="H24" s="6">
-        <f t="shared" si="0"/>
-        <v>5.82</v>
-      </c>
-      <c r="I24" s="6">
-        <f t="shared" si="0"/>
-        <v>1.52</v>
-      </c>
-      <c r="J24" s="6">
-        <f t="shared" si="0"/>
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="6">
-        <f>STDEV(B3:B22)</f>
-        <v>2.5037866060071998</v>
-      </c>
-      <c r="C25" s="6">
-        <f>STDEV(C3:C22)</f>
-        <v>1.2268380410418354</v>
-      </c>
-      <c r="D25" s="6">
-        <f>STDEV(D3:D22)</f>
-        <v>1.053452968999915</v>
-      </c>
-      <c r="E25" s="6">
-        <f t="shared" ref="E25:J25" si="1">STDEV(E3:E22)</f>
-        <v>2.6183311277867145</v>
-      </c>
-      <c r="F25" s="6">
-        <f t="shared" si="1"/>
-        <v>1.6560177344588152</v>
-      </c>
-      <c r="G25" s="6">
-        <f t="shared" si="1"/>
-        <v>1.2483568147136885</v>
-      </c>
-      <c r="H25" s="6">
-        <f t="shared" si="1"/>
-        <v>3.4266141029486121</v>
-      </c>
-      <c r="I25" s="6">
-        <f t="shared" si="1"/>
-        <v>1.10672584918902</v>
-      </c>
-      <c r="J25" s="6">
-        <f t="shared" si="1"/>
-        <v>1.1385124181649446</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="6">
-        <f>B24+B25*3</f>
-        <v>11.761359818021599</v>
-      </c>
-      <c r="C26" s="6">
-        <f t="shared" ref="C26:J26" si="2">C24+C25*3</f>
-        <v>5.1555141231255055</v>
-      </c>
-      <c r="D26" s="6">
-        <f t="shared" si="2"/>
-        <v>4.7253589069997455</v>
-      </c>
-      <c r="E26" s="6">
-        <f t="shared" si="2"/>
-        <v>11.779993383360143</v>
-      </c>
-      <c r="F26" s="6">
-        <f t="shared" si="2"/>
-        <v>7.5330532033764452</v>
-      </c>
-      <c r="G26" s="6">
-        <f t="shared" si="2"/>
-        <v>5.4400704441410657</v>
-      </c>
-      <c r="H26" s="6">
-        <f t="shared" si="2"/>
-        <v>16.099842308845837</v>
-      </c>
-      <c r="I26" s="6">
-        <f t="shared" si="2"/>
-        <v>4.8401775475670599</v>
-      </c>
-      <c r="J26" s="6">
-        <f t="shared" si="2"/>
-        <v>4.8755372544948337</v>
-      </c>
-      <c r="M26" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="N26" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="O26" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="P26" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q26" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="R26" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="U26" s="3"/>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="M27" s="12">
-        <v>4.25</v>
-      </c>
-      <c r="N27" s="12">
-        <v>2.5037866060071998</v>
-      </c>
-      <c r="O27" s="12">
-        <v>1.4749999999999999</v>
-      </c>
-      <c r="P27" s="12">
-        <v>1.2268380410418354</v>
-      </c>
-      <c r="Q27" s="12">
-        <v>1.5650000000000002</v>
-      </c>
-      <c r="R27" s="12">
-        <v>1.053452968999915</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
-      <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="L28" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="M28" s="12">
-        <v>3.9249999999999994</v>
-      </c>
-      <c r="N28" s="12">
-        <v>2.6183311277867145</v>
-      </c>
-      <c r="O28" s="12">
-        <v>2.5649999999999999</v>
-      </c>
-      <c r="P28" s="12">
-        <v>1.6560177344588152</v>
-      </c>
-      <c r="Q28" s="12">
-        <v>1.6949999999999998</v>
-      </c>
-      <c r="R28" s="12">
-        <v>1.2483568147136885</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="B29" s="6">
-        <f>MAX(B26,E26,H26)</f>
-        <v>16.099842308845837</v>
-      </c>
-      <c r="C29" s="6">
-        <f>MAX(C26,F26,I26)</f>
-        <v>7.5330532033764452</v>
-      </c>
-      <c r="D29" s="6">
-        <f>MAX(D26,G26,J26)</f>
-        <v>5.4400704441410657</v>
-      </c>
-      <c r="L29" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M29" s="12">
-        <v>5.82</v>
-      </c>
-      <c r="N29" s="12">
-        <v>3.4266141029486121</v>
-      </c>
-      <c r="O29" s="12">
-        <v>1.52</v>
-      </c>
-      <c r="P29" s="12">
-        <v>1.10672584918902</v>
-      </c>
-      <c r="Q29" s="12">
-        <v>1.46</v>
-      </c>
-      <c r="R29" s="12">
-        <v>1.1385124181649446</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="M31" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="N31" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="O31" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="P31" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q31" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="R31" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
-      <c r="E32" s="6"/>
-      <c r="L32" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="M32" s="12">
-        <f>M27</f>
-        <v>4.25</v>
-      </c>
-      <c r="N32" s="12">
-        <f t="shared" ref="N32:P32" si="3">N27</f>
-        <v>2.5037866060071998</v>
-      </c>
-      <c r="O32" s="12">
-        <f t="shared" si="3"/>
-        <v>1.4749999999999999</v>
-      </c>
-      <c r="P32" s="12">
-        <f t="shared" si="3"/>
-        <v>1.2268380410418354</v>
-      </c>
-      <c r="Q32" s="12">
-        <f t="shared" ref="Q32:R34" si="4">Q27*0.01745329251</f>
-        <v>2.7314402778150001E-2</v>
-      </c>
-      <c r="R32" s="12">
-        <f t="shared" si="4"/>
-        <v>1.8386222813483479E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="12:18">
-      <c r="L33" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="M33" s="12">
-        <f t="shared" ref="M33:P33" si="5">M28</f>
-        <v>3.9249999999999994</v>
-      </c>
-      <c r="N33" s="12">
-        <f t="shared" si="5"/>
-        <v>2.6183311277867145</v>
-      </c>
-      <c r="O33" s="12">
-        <f t="shared" si="5"/>
-        <v>2.5649999999999999</v>
-      </c>
-      <c r="P33" s="12">
-        <f t="shared" si="5"/>
-        <v>1.6560177344588152</v>
-      </c>
-      <c r="Q33" s="12">
-        <f t="shared" si="4"/>
-        <v>2.9583330804449998E-2</v>
-      </c>
-      <c r="R33" s="12">
-        <f t="shared" si="4"/>
-        <v>2.1787936644049877E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="12:18">
-      <c r="L34" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="M34" s="12">
-        <f t="shared" ref="M34:P34" si="6">M29</f>
-        <v>5.82</v>
-      </c>
-      <c r="N34" s="12">
-        <f t="shared" si="6"/>
-        <v>3.4266141029486121</v>
-      </c>
-      <c r="O34" s="12">
-        <f t="shared" si="6"/>
-        <v>1.52</v>
-      </c>
-      <c r="P34" s="12">
-        <f t="shared" si="6"/>
-        <v>1.10672584918902</v>
-      </c>
-      <c r="Q34" s="12">
-        <f t="shared" si="4"/>
-        <v>2.5481807064599998E-2</v>
-      </c>
-      <c r="R34" s="12">
-        <f t="shared" si="4"/>
-        <v>1.9870790260500214E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="12:18">
-      <c r="L35" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="M35" s="12">
-        <f>AVERAGE(M32:M34)</f>
-        <v>4.665</v>
-      </c>
-      <c r="N35" s="12">
-        <f t="shared" ref="N35:R35" si="7">AVERAGE(N32:N34)</f>
-        <v>2.8495772789141753</v>
-      </c>
-      <c r="O35" s="12">
-        <f t="shared" si="7"/>
-        <v>1.8533333333333335</v>
-      </c>
-      <c r="P35" s="12">
-        <f t="shared" si="7"/>
-        <v>1.3298605415632234</v>
-      </c>
-      <c r="Q35" s="12">
-        <f t="shared" si="7"/>
-        <v>2.74598468824E-2</v>
-      </c>
-      <c r="R35" s="12">
-        <f t="shared" si="7"/>
-        <v>2.0014983239344527E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R39"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35:R39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="B1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
@@ -18916,7 +18915,7 @@
       </c>
     </row>
     <row r="39" spans="12:18">
-      <c r="L39" s="20" t="s">
+      <c r="L39" s="18" t="s">
         <v>7</v>
       </c>
       <c r="M39" s="12">
@@ -18958,7 +18957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -19181,8 +19180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK53"/>
   <sheetViews>
-    <sheetView topLeftCell="V10" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3:AK10"/>
+    <sheetView topLeftCell="V1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -19454,43 +19453,43 @@
         <v>4</v>
       </c>
       <c r="X7" s="12">
-        <v>37.186069959183662</v>
+        <v>24.355517121775517</v>
       </c>
       <c r="Y7" s="12">
-        <v>14.850241997686163</v>
+        <v>17.472085512364</v>
       </c>
       <c r="Z7" s="12">
-        <v>183.2115121224478</v>
+        <v>138.65597546530731</v>
       </c>
       <c r="AA7" s="12">
-        <v>7.296972233069174</v>
+        <v>6.772731672518213</v>
       </c>
       <c r="AB7" s="12">
-        <v>115.84973551020366</v>
+        <v>42.796422130611809</v>
       </c>
       <c r="AC7" s="12">
-        <v>16.265329219752218</v>
+        <v>16.371628170412606</v>
       </c>
       <c r="AE7" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="AF7" s="12">
-        <v>37.186069959183662</v>
+        <v>24.355517121775517</v>
       </c>
       <c r="AG7" s="12">
-        <v>14.850241997686163</v>
+        <v>17.472085512364</v>
       </c>
       <c r="AH7" s="12">
-        <v>183.2115121224478</v>
+        <v>138.65597546530731</v>
       </c>
       <c r="AI7" s="12">
-        <v>7.296972233069174</v>
+        <v>6.772731672518213</v>
       </c>
       <c r="AJ7" s="12">
-        <v>115.84973551020366</v>
+        <v>42.796422130611809</v>
       </c>
       <c r="AK7" s="12">
-        <v>16.265329219752218</v>
+        <v>16.371628170412606</v>
       </c>
     </row>
     <row r="8" spans="1:37">
@@ -19519,43 +19518,43 @@
         <v>5</v>
       </c>
       <c r="X8" s="12">
-        <v>24.355517121775517</v>
+        <v>37.186069959183662</v>
       </c>
       <c r="Y8" s="12">
-        <v>17.472085512364</v>
+        <v>14.850241997686163</v>
       </c>
       <c r="Z8" s="12">
-        <v>138.65597546530731</v>
+        <v>183.2115121224478</v>
       </c>
       <c r="AA8" s="12">
-        <v>6.772731672518213</v>
+        <v>7.296972233069174</v>
       </c>
       <c r="AB8" s="12">
-        <v>42.796422130611809</v>
+        <v>115.84973551020366</v>
       </c>
       <c r="AC8" s="12">
-        <v>16.371628170412606</v>
+        <v>16.265329219752218</v>
       </c>
       <c r="AE8" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="AF8" s="12">
-        <v>24.355517121775517</v>
+        <v>37.186069959183662</v>
       </c>
       <c r="AG8" s="12">
-        <v>17.472085512364</v>
+        <v>14.850241997686163</v>
       </c>
       <c r="AH8" s="12">
-        <v>138.65597546530731</v>
+        <v>183.2115121224478</v>
       </c>
       <c r="AI8" s="12">
-        <v>6.772731672518213</v>
+        <v>7.296972233069174</v>
       </c>
       <c r="AJ8" s="12">
-        <v>42.796422130611809</v>
+        <v>115.84973551020366</v>
       </c>
       <c r="AK8" s="12">
-        <v>16.371628170412606</v>
+        <v>16.265329219752218</v>
       </c>
     </row>
     <row r="9" spans="1:37">
@@ -19629,15 +19628,15 @@
       </c>
       <c r="AH10" s="12">
         <f t="shared" si="0"/>
-        <v>126.36954109659943</v>
+        <v>126.36954109659945</v>
       </c>
       <c r="AI10" s="12">
         <f t="shared" si="0"/>
-        <v>8.0733355559358806</v>
+        <v>8.0733355559358824</v>
       </c>
       <c r="AJ10" s="12">
         <f t="shared" si="0"/>
-        <v>117.6091874897955</v>
+        <v>117.60918748979549</v>
       </c>
       <c r="AK10" s="12">
         <f t="shared" si="0"/>
@@ -19645,30 +19644,30 @@
       </c>
     </row>
     <row r="11" spans="1:37">
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19" t="s">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19" t="s">
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
     </row>
     <row r="12" spans="1:37">
       <c r="D12" s="10" t="s">
@@ -20199,30 +20198,30 @@
       <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19" t="s">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19" t="s">
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="20"/>
     </row>
     <row r="28" spans="1:21">
       <c r="D28" s="10" t="s">
@@ -21131,8 +21130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X247"/>
   <sheetViews>
-    <sheetView topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="J249" sqref="J249"/>
+    <sheetView topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="H260" sqref="H260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34940,8 +34939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4:AC8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -35160,30 +35159,30 @@
       </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19" t="s">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19" t="s">
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
     </row>
     <row r="12" spans="1:29">
       <c r="D12" s="10" t="s">
@@ -35815,7 +35814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L248"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L249" sqref="L249"/>
     </sheetView>
   </sheetViews>
@@ -42984,7 +42983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="X32" sqref="X32:AD37"/>
     </sheetView>
   </sheetViews>

</xml_diff>